<commit_message>
updates to routes, quizzable questions update functional
</commit_message>
<xml_diff>
--- a/seed.xlsx
+++ b/seed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="4" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="359">
   <si>
     <t>id</t>
   </si>
@@ -1133,6 +1133,12 @@
   </si>
   <si>
     <t>REACTJS FILLER FACT - 1</t>
+  </si>
+  <si>
+    <t>What are HTML elements represented by?</t>
+  </si>
+  <si>
+    <t>Tags</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1220,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="190">
+  <cellStyleXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1405,6 +1411,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1426,7 +1450,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="181"/>
   </cellXfs>
-  <cellStyles count="190">
+  <cellStyles count="208">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1525,6 +1549,24 @@
     <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1935,7 +1977,8 @@
   <dimension ref="C2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H20"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2291,8 +2334,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3249,7 +3294,8 @@
   <dimension ref="C2:H207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H207"/>
+      <pane ySplit="2" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:H207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7481,9 +7527,8 @@
       <c r="C205" s="2">
         <v>203</v>
       </c>
-      <c r="D205" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>Filler Answer 203</v>
+      <c r="D205" s="3" t="s">
+        <v>358</v>
       </c>
       <c r="E205" s="2" t="s">
         <v>96</v>
@@ -7495,7 +7540,7 @@
         <v>34</v>
       </c>
       <c r="H205" s="2">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="206" spans="3:8" x14ac:dyDescent="0.2">
@@ -7548,10 +7593,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J206"/>
+  <dimension ref="B3:J207"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:J206"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7612,7 +7658,9 @@
       <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
       <c r="I4" s="2">
         <v>3</v>
       </c>
@@ -7639,7 +7687,9 @@
       <c r="G5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
       <c r="I5" s="2">
         <v>3</v>
       </c>
@@ -7666,7 +7716,9 @@
       <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
       <c r="I6" s="2">
         <v>3</v>
       </c>
@@ -7693,7 +7745,9 @@
       <c r="G7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
       <c r="I7" s="2">
         <v>3</v>
       </c>
@@ -7720,7 +7774,9 @@
       <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
       <c r="I8" s="2">
         <v>3</v>
       </c>
@@ -7747,7 +7803,9 @@
       <c r="G9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
       <c r="I9" s="2">
         <v>3</v>
       </c>
@@ -7774,7 +7832,9 @@
       <c r="G10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
       <c r="I10" s="2">
         <v>3</v>
       </c>
@@ -7801,7 +7861,9 @@
       <c r="G11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
       <c r="I11" s="2">
         <v>3</v>
       </c>
@@ -7828,7 +7890,9 @@
       <c r="G12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
       <c r="I12" s="2">
         <v>3</v>
       </c>
@@ -7855,7 +7919,9 @@
       <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
       <c r="I13" s="2">
         <v>3</v>
       </c>
@@ -7882,7 +7948,9 @@
       <c r="G14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
       <c r="I14" s="2">
         <v>3</v>
       </c>
@@ -7909,7 +7977,9 @@
       <c r="G15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
       <c r="I15" s="2">
         <v>3</v>
       </c>
@@ -7936,7 +8006,9 @@
       <c r="G16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
       <c r="I16" s="2">
         <v>3</v>
       </c>
@@ -7963,7 +8035,9 @@
       <c r="G17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>3</v>
+      </c>
       <c r="I17" s="2">
         <v>3</v>
       </c>
@@ -7990,7 +8064,9 @@
       <c r="G18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>3</v>
+      </c>
       <c r="I18" s="2">
         <v>3</v>
       </c>
@@ -8017,7 +8093,9 @@
       <c r="G19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>4</v>
+      </c>
       <c r="I19" s="2">
         <v>3</v>
       </c>
@@ -8044,7 +8122,9 @@
       <c r="G20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>4</v>
+      </c>
       <c r="I20" s="2">
         <v>3</v>
       </c>
@@ -8071,7 +8151,9 @@
       <c r="G21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>4</v>
+      </c>
       <c r="I21" s="2">
         <v>3</v>
       </c>
@@ -8098,7 +8180,9 @@
       <c r="G22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>4</v>
+      </c>
       <c r="I22" s="2">
         <v>3</v>
       </c>
@@ -8125,7 +8209,9 @@
       <c r="G23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2">
+        <v>4</v>
+      </c>
       <c r="I23" s="2">
         <v>9</v>
       </c>
@@ -8152,7 +8238,9 @@
       <c r="G24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2">
+        <v>5</v>
+      </c>
       <c r="I24" s="2">
         <v>9</v>
       </c>
@@ -8179,7 +8267,9 @@
       <c r="G25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2">
+        <v>5</v>
+      </c>
       <c r="I25" s="2">
         <v>9</v>
       </c>
@@ -8206,7 +8296,9 @@
       <c r="G26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2">
+        <v>5</v>
+      </c>
       <c r="I26" s="2">
         <v>9</v>
       </c>
@@ -8233,7 +8325,9 @@
       <c r="G27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2">
+        <v>5</v>
+      </c>
       <c r="I27" s="2">
         <v>9</v>
       </c>
@@ -8260,7 +8354,9 @@
       <c r="G28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="2"/>
+      <c r="H28" s="2">
+        <v>5</v>
+      </c>
       <c r="I28" s="2">
         <v>9</v>
       </c>
@@ -8287,7 +8383,9 @@
       <c r="G29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H29" s="2"/>
+      <c r="H29" s="2">
+        <v>6</v>
+      </c>
       <c r="I29" s="2">
         <v>10</v>
       </c>
@@ -8314,7 +8412,9 @@
       <c r="G30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H30" s="2"/>
+      <c r="H30" s="2">
+        <v>6</v>
+      </c>
       <c r="I30" s="2">
         <v>10</v>
       </c>
@@ -8341,7 +8441,9 @@
       <c r="G31" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="2">
+        <v>6</v>
+      </c>
       <c r="I31" s="2">
         <v>10</v>
       </c>
@@ -8368,7 +8470,9 @@
       <c r="G32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="2"/>
+      <c r="H32" s="2">
+        <v>6</v>
+      </c>
       <c r="I32" s="2">
         <v>10</v>
       </c>
@@ -8395,7 +8499,9 @@
       <c r="G33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2">
+        <v>6</v>
+      </c>
       <c r="I33" s="2">
         <v>10</v>
       </c>
@@ -8422,7 +8528,9 @@
       <c r="G34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="2"/>
+      <c r="H34" s="2">
+        <v>7</v>
+      </c>
       <c r="I34" s="2">
         <v>10</v>
       </c>
@@ -8449,7 +8557,9 @@
       <c r="G35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="2"/>
+      <c r="H35" s="2">
+        <v>7</v>
+      </c>
       <c r="I35" s="2">
         <v>10</v>
       </c>
@@ -8476,7 +8586,9 @@
       <c r="G36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2">
+        <v>7</v>
+      </c>
       <c r="I36" s="2">
         <v>10</v>
       </c>
@@ -8503,7 +8615,9 @@
       <c r="G37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="2">
+        <v>7</v>
+      </c>
       <c r="I37" s="2">
         <v>10</v>
       </c>
@@ -8530,7 +8644,9 @@
       <c r="G38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2">
+        <v>7</v>
+      </c>
       <c r="I38" s="2">
         <v>10</v>
       </c>
@@ -8557,7 +8673,9 @@
       <c r="G39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H39" s="2"/>
+      <c r="H39" s="2">
+        <v>7</v>
+      </c>
       <c r="I39" s="2">
         <v>10</v>
       </c>
@@ -8584,7 +8702,9 @@
       <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="2"/>
+      <c r="H40" s="2">
+        <v>8</v>
+      </c>
       <c r="I40" s="2">
         <v>4</v>
       </c>
@@ -8611,7 +8731,9 @@
       <c r="G41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H41" s="2"/>
+      <c r="H41" s="2">
+        <v>8</v>
+      </c>
       <c r="I41" s="2">
         <v>4</v>
       </c>
@@ -8638,7 +8760,9 @@
       <c r="G42" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H42" s="2"/>
+      <c r="H42" s="2">
+        <v>8</v>
+      </c>
       <c r="I42" s="2">
         <v>4</v>
       </c>
@@ -8665,7 +8789,9 @@
       <c r="G43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H43" s="2"/>
+      <c r="H43" s="2">
+        <v>8</v>
+      </c>
       <c r="I43" s="2">
         <v>4</v>
       </c>
@@ -8692,7 +8818,9 @@
       <c r="G44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H44" s="2"/>
+      <c r="H44" s="2">
+        <v>8</v>
+      </c>
       <c r="I44" s="2">
         <v>4</v>
       </c>
@@ -8719,7 +8847,9 @@
       <c r="G45" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2">
+        <v>8</v>
+      </c>
       <c r="I45" s="2">
         <v>4</v>
       </c>
@@ -8746,7 +8876,9 @@
       <c r="G46" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H46" s="2"/>
+      <c r="H46" s="2">
+        <v>9</v>
+      </c>
       <c r="I46" s="2">
         <v>4</v>
       </c>
@@ -8773,7 +8905,9 @@
       <c r="G47" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="2"/>
+      <c r="H47" s="2">
+        <v>9</v>
+      </c>
       <c r="I47" s="2">
         <v>3</v>
       </c>
@@ -8800,7 +8934,9 @@
       <c r="G48" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H48" s="8"/>
+      <c r="H48" s="8">
+        <v>9</v>
+      </c>
       <c r="I48" s="8">
         <v>1</v>
       </c>
@@ -8827,7 +8963,9 @@
       <c r="G49" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2">
+        <v>9</v>
+      </c>
       <c r="I49" s="2">
         <v>2</v>
       </c>
@@ -8854,7 +8992,9 @@
       <c r="G50" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H50" s="2"/>
+      <c r="H50" s="2">
+        <v>9</v>
+      </c>
       <c r="I50" s="2">
         <v>12</v>
       </c>
@@ -8881,7 +9021,9 @@
       <c r="G51" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="2"/>
+      <c r="H51" s="2">
+        <v>9</v>
+      </c>
       <c r="I51" s="2">
         <v>10</v>
       </c>
@@ -8908,7 +9050,9 @@
       <c r="G52" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H52" s="2"/>
+      <c r="H52" s="2">
+        <v>10</v>
+      </c>
       <c r="I52" s="2">
         <v>5</v>
       </c>
@@ -13072,6 +13216,35 @@
       </c>
       <c r="J206" s="2">
         <v>202</v>
+      </c>
+    </row>
+    <row r="207" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B207" s="2">
+        <v>204</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D207" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H207">
+        <v>3</v>
+      </c>
+      <c r="I207" s="2">
+        <v>1</v>
+      </c>
+      <c r="J207" s="2">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -13085,7 +13258,8 @@
   <dimension ref="B3:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H8"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13204,1431 +13378,1219 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G73"/>
+  <dimension ref="B3:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G73"/>
+      <pane ySplit="3" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="b">
         <v>0</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>34</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="b">
         <v>0</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>34</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
-        <v>34</v>
+      <c r="E5">
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="b">
         <v>0</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
+      <c r="E6">
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="b">
         <v>0</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
-        <v>34</v>
+      <c r="E7">
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="b">
         <v>0</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>34</v>
+      <c r="E8">
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="b">
         <v>0</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>34</v>
       </c>
       <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
+      <c r="E9">
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="b">
         <v>0</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" t="s">
-        <v>34</v>
+      <c r="E10">
+        <v>7</v>
       </c>
       <c r="F10">
-        <v>7</v>
-      </c>
-      <c r="G10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="b">
         <v>0</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>34</v>
+      <c r="E11">
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>8</v>
-      </c>
-      <c r="G11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="b">
         <v>0</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>34</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
-        <v>34</v>
+      <c r="E12">
+        <v>9</v>
       </c>
       <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="b">
         <v>0</v>
       </c>
-      <c r="C13" t="b">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
-        <v>34</v>
+      <c r="E13">
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="b">
         <v>0</v>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>34</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
-        <v>34</v>
+      <c r="E14">
+        <v>11</v>
       </c>
       <c r="F14">
-        <v>11</v>
-      </c>
-      <c r="G14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="b">
         <v>0</v>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="E15" t="s">
-        <v>34</v>
+      <c r="E15">
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="b">
         <v>0</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" t="s">
-        <v>34</v>
+      <c r="E16">
+        <v>13</v>
       </c>
       <c r="F16">
-        <v>13</v>
-      </c>
-      <c r="G16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="b">
         <v>0</v>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>34</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
       </c>
-      <c r="E17" t="s">
-        <v>34</v>
+      <c r="E17">
+        <v>14</v>
       </c>
       <c r="F17">
-        <v>14</v>
-      </c>
-      <c r="G17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="b">
         <v>0</v>
       </c>
-      <c r="C18" t="b">
-        <v>0</v>
+      <c r="C18" t="s">
+        <v>34</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
-        <v>34</v>
+      <c r="E18">
+        <v>15</v>
       </c>
       <c r="F18">
-        <v>15</v>
-      </c>
-      <c r="G18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="b">
         <v>0</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
+      <c r="C19" t="s">
+        <v>34</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
-        <v>34</v>
+      <c r="E19">
+        <v>16</v>
       </c>
       <c r="F19">
-        <v>16</v>
-      </c>
-      <c r="G19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="b">
         <v>0</v>
       </c>
-      <c r="C20" t="b">
-        <v>0</v>
+      <c r="C20" t="s">
+        <v>34</v>
       </c>
       <c r="D20" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
-        <v>34</v>
+      <c r="E20">
+        <v>17</v>
       </c>
       <c r="F20">
-        <v>17</v>
-      </c>
-      <c r="G20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="b">
         <v>0</v>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
+      <c r="C21" t="s">
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
       </c>
-      <c r="E21" t="s">
-        <v>34</v>
+      <c r="E21">
+        <v>18</v>
       </c>
       <c r="F21">
-        <v>18</v>
-      </c>
-      <c r="G21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="b">
         <v>0</v>
       </c>
-      <c r="C22" t="b">
-        <v>0</v>
+      <c r="C22" t="s">
+        <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
       </c>
-      <c r="E22" t="s">
-        <v>34</v>
+      <c r="E22">
+        <v>19</v>
       </c>
       <c r="F22">
-        <v>19</v>
-      </c>
-      <c r="G22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="b">
         <v>0</v>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
+      <c r="C23" t="s">
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="E23" t="s">
-        <v>34</v>
+      <c r="E23">
+        <v>20</v>
       </c>
       <c r="F23">
-        <v>20</v>
-      </c>
-      <c r="G23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="b">
         <v>0</v>
       </c>
-      <c r="C24" t="b">
-        <v>0</v>
+      <c r="C24" t="s">
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>34</v>
       </c>
-      <c r="E24" t="s">
-        <v>34</v>
+      <c r="E24">
+        <v>21</v>
       </c>
       <c r="F24">
-        <v>21</v>
-      </c>
-      <c r="G24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="b">
         <v>0</v>
       </c>
-      <c r="C25" t="b">
-        <v>0</v>
+      <c r="C25" t="s">
+        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="E25" t="s">
-        <v>34</v>
+      <c r="E25">
+        <v>22</v>
       </c>
       <c r="F25">
-        <v>22</v>
-      </c>
-      <c r="G25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="b">
         <v>0</v>
       </c>
-      <c r="C26" t="b">
-        <v>0</v>
+      <c r="C26" t="s">
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
       </c>
-      <c r="E26" t="s">
-        <v>34</v>
+      <c r="E26">
+        <v>23</v>
       </c>
       <c r="F26">
-        <v>23</v>
-      </c>
-      <c r="G26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="b">
         <v>0</v>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
+      <c r="C27" t="s">
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>34</v>
       </c>
-      <c r="E27" t="s">
-        <v>34</v>
+      <c r="E27">
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>24</v>
-      </c>
-      <c r="G27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="b">
         <v>0</v>
       </c>
-      <c r="C28" t="b">
-        <v>0</v>
+      <c r="C28" t="s">
+        <v>34</v>
       </c>
       <c r="D28" t="s">
         <v>34</v>
       </c>
-      <c r="E28" t="s">
-        <v>34</v>
+      <c r="E28">
+        <v>25</v>
       </c>
       <c r="F28">
-        <v>25</v>
-      </c>
-      <c r="G28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="b">
         <v>0</v>
       </c>
-      <c r="C29" t="b">
-        <v>0</v>
+      <c r="C29" t="s">
+        <v>34</v>
       </c>
       <c r="D29" t="s">
         <v>34</v>
       </c>
-      <c r="E29" t="s">
-        <v>34</v>
+      <c r="E29">
+        <v>26</v>
       </c>
       <c r="F29">
-        <v>26</v>
-      </c>
-      <c r="G29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="b">
         <v>0</v>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
+      <c r="C30" t="s">
+        <v>34</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
       </c>
-      <c r="E30" t="s">
-        <v>34</v>
+      <c r="E30">
+        <v>27</v>
       </c>
       <c r="F30">
-        <v>27</v>
-      </c>
-      <c r="G30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="b">
         <v>0</v>
       </c>
-      <c r="C31" t="b">
-        <v>0</v>
+      <c r="C31" t="s">
+        <v>34</v>
       </c>
       <c r="D31" t="s">
         <v>34</v>
       </c>
-      <c r="E31" t="s">
-        <v>34</v>
+      <c r="E31">
+        <v>28</v>
       </c>
       <c r="F31">
-        <v>28</v>
-      </c>
-      <c r="G31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="b">
         <v>0</v>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
+      <c r="C32" t="s">
+        <v>34</v>
       </c>
       <c r="D32" t="s">
         <v>34</v>
       </c>
-      <c r="E32" t="s">
-        <v>34</v>
+      <c r="E32">
+        <v>29</v>
       </c>
       <c r="F32">
-        <v>29</v>
-      </c>
-      <c r="G32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="b">
         <v>0</v>
       </c>
-      <c r="C33" t="b">
-        <v>0</v>
+      <c r="C33" t="s">
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>34</v>
       </c>
-      <c r="E33" t="s">
-        <v>34</v>
+      <c r="E33">
+        <v>30</v>
       </c>
       <c r="F33">
-        <v>30</v>
-      </c>
-      <c r="G33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="b">
         <v>0</v>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
+      <c r="C34" t="s">
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
       </c>
-      <c r="E34" t="s">
-        <v>34</v>
+      <c r="E34">
+        <v>31</v>
       </c>
       <c r="F34">
-        <v>31</v>
-      </c>
-      <c r="G34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="b">
         <v>0</v>
       </c>
-      <c r="C35" t="b">
-        <v>0</v>
+      <c r="C35" t="s">
+        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>34</v>
       </c>
-      <c r="E35" t="s">
-        <v>34</v>
+      <c r="E35">
+        <v>32</v>
       </c>
       <c r="F35">
-        <v>32</v>
-      </c>
-      <c r="G35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="b">
         <v>0</v>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
+      <c r="C36" t="s">
+        <v>34</v>
       </c>
       <c r="D36" t="s">
         <v>34</v>
       </c>
-      <c r="E36" t="s">
-        <v>34</v>
+      <c r="E36">
+        <v>33</v>
       </c>
       <c r="F36">
-        <v>33</v>
-      </c>
-      <c r="G36">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="b">
         <v>0</v>
       </c>
-      <c r="C37" t="b">
-        <v>0</v>
+      <c r="C37" t="s">
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>34</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37">
         <v>34</v>
       </c>
       <c r="F37">
-        <v>34</v>
-      </c>
-      <c r="G37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="b">
         <v>0</v>
       </c>
-      <c r="C38" t="b">
-        <v>0</v>
+      <c r="C38" t="s">
+        <v>34</v>
       </c>
       <c r="D38" t="s">
         <v>34</v>
       </c>
-      <c r="E38" t="s">
-        <v>34</v>
+      <c r="E38">
+        <v>35</v>
       </c>
       <c r="F38">
-        <v>35</v>
-      </c>
-      <c r="G38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="b">
         <v>0</v>
       </c>
-      <c r="C39" t="b">
-        <v>0</v>
+      <c r="C39" t="s">
+        <v>34</v>
       </c>
       <c r="D39" t="s">
         <v>34</v>
       </c>
-      <c r="E39" t="s">
-        <v>34</v>
+      <c r="E39">
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="b">
         <v>0</v>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
+      <c r="C40" t="s">
+        <v>34</v>
       </c>
       <c r="D40" t="s">
         <v>34</v>
       </c>
-      <c r="E40" t="s">
-        <v>34</v>
+      <c r="E40">
+        <v>2</v>
       </c>
       <c r="F40">
         <v>2</v>
       </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="b">
         <v>0</v>
       </c>
-      <c r="C41" t="b">
-        <v>0</v>
+      <c r="C41" t="s">
+        <v>34</v>
       </c>
       <c r="D41" t="s">
         <v>34</v>
       </c>
-      <c r="E41" t="s">
-        <v>34</v>
+      <c r="E41">
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>3</v>
-      </c>
-      <c r="G41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="b">
         <v>0</v>
       </c>
-      <c r="C42" t="b">
-        <v>0</v>
+      <c r="C42" t="s">
+        <v>34</v>
       </c>
       <c r="D42" t="s">
         <v>34</v>
       </c>
-      <c r="E42" t="s">
-        <v>34</v>
+      <c r="E42">
+        <v>4</v>
       </c>
       <c r="F42">
-        <v>4</v>
-      </c>
-      <c r="G42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="b">
         <v>0</v>
       </c>
-      <c r="C43" t="b">
-        <v>0</v>
+      <c r="C43" t="s">
+        <v>34</v>
       </c>
       <c r="D43" t="s">
         <v>34</v>
       </c>
-      <c r="E43" t="s">
-        <v>34</v>
+      <c r="E43">
+        <v>5</v>
       </c>
       <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="b">
         <v>0</v>
       </c>
-      <c r="C44" t="b">
-        <v>0</v>
+      <c r="C44" t="s">
+        <v>34</v>
       </c>
       <c r="D44" t="s">
         <v>34</v>
       </c>
-      <c r="E44" t="s">
-        <v>34</v>
+      <c r="E44">
+        <v>6</v>
       </c>
       <c r="F44">
-        <v>6</v>
-      </c>
-      <c r="G44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="b">
         <v>0</v>
       </c>
-      <c r="C45" t="b">
-        <v>0</v>
+      <c r="C45" t="s">
+        <v>34</v>
       </c>
       <c r="D45" t="s">
         <v>34</v>
       </c>
-      <c r="E45" t="s">
-        <v>34</v>
+      <c r="E45">
+        <v>7</v>
       </c>
       <c r="F45">
-        <v>7</v>
-      </c>
-      <c r="G45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="b">
         <v>0</v>
       </c>
-      <c r="C46" t="b">
-        <v>0</v>
+      <c r="C46" t="s">
+        <v>34</v>
       </c>
       <c r="D46" t="s">
         <v>34</v>
       </c>
-      <c r="E46" t="s">
-        <v>34</v>
+      <c r="E46">
+        <v>8</v>
       </c>
       <c r="F46">
-        <v>8</v>
-      </c>
-      <c r="G46">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="b">
         <v>0</v>
       </c>
-      <c r="C47" t="b">
-        <v>0</v>
+      <c r="C47" t="s">
+        <v>34</v>
       </c>
       <c r="D47" t="s">
         <v>34</v>
       </c>
-      <c r="E47" t="s">
-        <v>34</v>
+      <c r="E47">
+        <v>9</v>
       </c>
       <c r="F47">
-        <v>9</v>
-      </c>
-      <c r="G47">
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="b">
         <v>0</v>
       </c>
-      <c r="C48" t="b">
-        <v>0</v>
+      <c r="C48" t="s">
+        <v>34</v>
       </c>
       <c r="D48" t="s">
         <v>34</v>
       </c>
-      <c r="E48" t="s">
-        <v>34</v>
+      <c r="E48">
+        <v>10</v>
       </c>
       <c r="F48">
-        <v>10</v>
-      </c>
-      <c r="G48">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="b">
         <v>0</v>
       </c>
-      <c r="C49" t="b">
-        <v>0</v>
+      <c r="C49" t="s">
+        <v>34</v>
       </c>
       <c r="D49" t="s">
         <v>34</v>
       </c>
-      <c r="E49" t="s">
-        <v>34</v>
+      <c r="E49">
+        <v>11</v>
       </c>
       <c r="F49">
-        <v>11</v>
-      </c>
-      <c r="G49">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="b">
         <v>0</v>
       </c>
-      <c r="C50" t="b">
-        <v>0</v>
+      <c r="C50" t="s">
+        <v>34</v>
       </c>
       <c r="D50" t="s">
         <v>34</v>
       </c>
-      <c r="E50" t="s">
-        <v>34</v>
+      <c r="E50">
+        <v>12</v>
       </c>
       <c r="F50">
-        <v>12</v>
-      </c>
-      <c r="G50">
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="b">
         <v>0</v>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
+      <c r="C51" t="s">
+        <v>34</v>
       </c>
       <c r="D51" t="s">
         <v>34</v>
       </c>
-      <c r="E51" t="s">
-        <v>34</v>
+      <c r="E51">
+        <v>13</v>
       </c>
       <c r="F51">
-        <v>13</v>
-      </c>
-      <c r="G51">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="b">
         <v>0</v>
       </c>
-      <c r="C52" t="b">
-        <v>0</v>
+      <c r="C52" t="s">
+        <v>34</v>
       </c>
       <c r="D52" t="s">
         <v>34</v>
       </c>
-      <c r="E52" t="s">
-        <v>34</v>
+      <c r="E52">
+        <v>14</v>
       </c>
       <c r="F52">
-        <v>14</v>
-      </c>
-      <c r="G52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="b">
         <v>0</v>
       </c>
-      <c r="C53" t="b">
-        <v>0</v>
+      <c r="C53" t="s">
+        <v>34</v>
       </c>
       <c r="D53" t="s">
         <v>34</v>
       </c>
-      <c r="E53" t="s">
-        <v>34</v>
+      <c r="E53">
+        <v>15</v>
       </c>
       <c r="F53">
-        <v>15</v>
-      </c>
-      <c r="G53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="b">
         <v>0</v>
       </c>
-      <c r="C54" t="b">
-        <v>0</v>
+      <c r="C54" t="s">
+        <v>34</v>
       </c>
       <c r="D54" t="s">
         <v>34</v>
       </c>
-      <c r="E54" t="s">
-        <v>34</v>
+      <c r="E54">
+        <v>16</v>
       </c>
       <c r="F54">
-        <v>16</v>
-      </c>
-      <c r="G54">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="b">
         <v>0</v>
       </c>
-      <c r="C55" t="b">
-        <v>0</v>
+      <c r="C55" t="s">
+        <v>34</v>
       </c>
       <c r="D55" t="s">
         <v>34</v>
       </c>
-      <c r="E55" t="s">
-        <v>34</v>
+      <c r="E55">
+        <v>17</v>
       </c>
       <c r="F55">
-        <v>17</v>
-      </c>
-      <c r="G55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" t="b">
         <v>0</v>
       </c>
-      <c r="C56" t="b">
-        <v>0</v>
+      <c r="C56" t="s">
+        <v>34</v>
       </c>
       <c r="D56" t="s">
         <v>34</v>
       </c>
-      <c r="E56" t="s">
-        <v>34</v>
+      <c r="E56">
+        <v>18</v>
       </c>
       <c r="F56">
-        <v>18</v>
-      </c>
-      <c r="G56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" t="b">
         <v>0</v>
       </c>
-      <c r="C57" t="b">
-        <v>0</v>
+      <c r="C57" t="s">
+        <v>34</v>
       </c>
       <c r="D57" t="s">
         <v>34</v>
       </c>
-      <c r="E57" t="s">
-        <v>34</v>
+      <c r="E57">
+        <v>19</v>
       </c>
       <c r="F57">
-        <v>19</v>
-      </c>
-      <c r="G57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" t="b">
         <v>0</v>
       </c>
-      <c r="C58" t="b">
-        <v>0</v>
+      <c r="C58" t="s">
+        <v>34</v>
       </c>
       <c r="D58" t="s">
         <v>34</v>
       </c>
-      <c r="E58" t="s">
-        <v>34</v>
+      <c r="E58">
+        <v>20</v>
       </c>
       <c r="F58">
-        <v>20</v>
-      </c>
-      <c r="G58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" t="b">
         <v>0</v>
       </c>
-      <c r="C59" t="b">
-        <v>0</v>
+      <c r="C59" t="s">
+        <v>34</v>
       </c>
       <c r="D59" t="s">
         <v>34</v>
       </c>
-      <c r="E59" t="s">
-        <v>34</v>
+      <c r="E59">
+        <v>21</v>
       </c>
       <c r="F59">
-        <v>21</v>
-      </c>
-      <c r="G59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="b">
         <v>0</v>
       </c>
-      <c r="C60" t="b">
-        <v>0</v>
+      <c r="C60" t="s">
+        <v>34</v>
       </c>
       <c r="D60" t="s">
         <v>34</v>
       </c>
-      <c r="E60" t="s">
-        <v>34</v>
+      <c r="E60">
+        <v>22</v>
       </c>
       <c r="F60">
-        <v>22</v>
-      </c>
-      <c r="G60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" t="b">
         <v>0</v>
       </c>
-      <c r="C61" t="b">
-        <v>0</v>
+      <c r="C61" t="s">
+        <v>34</v>
       </c>
       <c r="D61" t="s">
         <v>34</v>
       </c>
-      <c r="E61" t="s">
-        <v>34</v>
+      <c r="E61">
+        <v>23</v>
       </c>
       <c r="F61">
-        <v>23</v>
-      </c>
-      <c r="G61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" t="b">
         <v>0</v>
       </c>
-      <c r="C62" t="b">
-        <v>0</v>
+      <c r="C62" t="s">
+        <v>34</v>
       </c>
       <c r="D62" t="s">
         <v>34</v>
       </c>
-      <c r="E62" t="s">
-        <v>34</v>
+      <c r="E62">
+        <v>24</v>
       </c>
       <c r="F62">
-        <v>24</v>
-      </c>
-      <c r="G62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" t="b">
         <v>0</v>
       </c>
-      <c r="C63" t="b">
-        <v>0</v>
+      <c r="C63" t="s">
+        <v>34</v>
       </c>
       <c r="D63" t="s">
         <v>34</v>
       </c>
-      <c r="E63" t="s">
-        <v>34</v>
+      <c r="E63">
+        <v>25</v>
       </c>
       <c r="F63">
-        <v>25</v>
-      </c>
-      <c r="G63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" t="b">
         <v>0</v>
       </c>
-      <c r="C64" t="b">
-        <v>0</v>
+      <c r="C64" t="s">
+        <v>34</v>
       </c>
       <c r="D64" t="s">
         <v>34</v>
       </c>
-      <c r="E64" t="s">
-        <v>34</v>
+      <c r="E64">
+        <v>26</v>
       </c>
       <c r="F64">
-        <v>26</v>
-      </c>
-      <c r="G64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B65" t="b">
         <v>0</v>
       </c>
-      <c r="C65" t="b">
-        <v>0</v>
+      <c r="C65" t="s">
+        <v>34</v>
       </c>
       <c r="D65" t="s">
         <v>34</v>
       </c>
-      <c r="E65" t="s">
-        <v>34</v>
+      <c r="E65">
+        <v>27</v>
       </c>
       <c r="F65">
-        <v>27</v>
-      </c>
-      <c r="G65">
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B66" t="b">
         <v>0</v>
       </c>
-      <c r="C66" t="b">
-        <v>0</v>
+      <c r="C66" t="s">
+        <v>34</v>
       </c>
       <c r="D66" t="s">
         <v>34</v>
       </c>
-      <c r="E66" t="s">
-        <v>34</v>
+      <c r="E66">
+        <v>28</v>
       </c>
       <c r="F66">
-        <v>28</v>
-      </c>
-      <c r="G66">
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B67" t="b">
         <v>0</v>
       </c>
-      <c r="C67" t="b">
-        <v>0</v>
+      <c r="C67" t="s">
+        <v>34</v>
       </c>
       <c r="D67" t="s">
         <v>34</v>
       </c>
-      <c r="E67" t="s">
-        <v>34</v>
+      <c r="E67">
+        <v>29</v>
       </c>
       <c r="F67">
-        <v>29</v>
-      </c>
-      <c r="G67">
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B68" t="b">
         <v>0</v>
       </c>
-      <c r="C68" t="b">
-        <v>0</v>
+      <c r="C68" t="s">
+        <v>34</v>
       </c>
       <c r="D68" t="s">
         <v>34</v>
       </c>
-      <c r="E68" t="s">
-        <v>34</v>
+      <c r="E68">
+        <v>30</v>
       </c>
       <c r="F68">
-        <v>30</v>
-      </c>
-      <c r="G68">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B69" t="b">
         <v>0</v>
       </c>
-      <c r="C69" t="b">
-        <v>0</v>
+      <c r="C69" t="s">
+        <v>34</v>
       </c>
       <c r="D69" t="s">
         <v>34</v>
       </c>
-      <c r="E69" t="s">
-        <v>34</v>
+      <c r="E69">
+        <v>31</v>
       </c>
       <c r="F69">
-        <v>31</v>
-      </c>
-      <c r="G69">
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B70" t="b">
         <v>0</v>
       </c>
-      <c r="C70" t="b">
-        <v>0</v>
+      <c r="C70" t="s">
+        <v>34</v>
       </c>
       <c r="D70" t="s">
         <v>34</v>
       </c>
-      <c r="E70" t="s">
-        <v>34</v>
+      <c r="E70">
+        <v>32</v>
       </c>
       <c r="F70">
-        <v>32</v>
-      </c>
-      <c r="G70">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B71" t="b">
         <v>0</v>
       </c>
-      <c r="C71" t="b">
-        <v>0</v>
+      <c r="C71" t="s">
+        <v>34</v>
       </c>
       <c r="D71" t="s">
         <v>34</v>
       </c>
-      <c r="E71" t="s">
-        <v>34</v>
+      <c r="E71">
+        <v>33</v>
       </c>
       <c r="F71">
-        <v>33</v>
-      </c>
-      <c r="G71">
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B72" t="b">
         <v>0</v>
       </c>
-      <c r="C72" t="b">
-        <v>0</v>
+      <c r="C72" t="s">
+        <v>34</v>
       </c>
       <c r="D72" t="s">
         <v>34</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72">
         <v>34</v>
       </c>
       <c r="F72">
-        <v>34</v>
-      </c>
-      <c r="G72">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" t="b">
         <v>0</v>
       </c>
-      <c r="C73" t="b">
-        <v>0</v>
+      <c r="C73" t="s">
+        <v>34</v>
       </c>
       <c r="D73" t="s">
         <v>34</v>
       </c>
-      <c r="E73" t="s">
-        <v>34</v>
+      <c r="E73">
+        <v>35</v>
       </c>
       <c r="F73">
-        <v>35</v>
-      </c>
-      <c r="G73">
         <v>2</v>
       </c>
     </row>
@@ -14640,724 +14602,818 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H33"/>
+  <dimension ref="B3:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H33"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>339</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>34</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>34</v>
-      </c>
       <c r="E5" t="s">
         <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>0.2</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7">
         <v>0.8</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
       <c r="E7" t="s">
         <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8">
         <v>0.60000000000000009</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" t="s">
         <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8">
         <v>5</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>34</v>
-      </c>
       <c r="E9" t="s">
         <v>34</v>
       </c>
       <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9">
         <v>6</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10">
         <v>0.60000000000000009</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
       <c r="E10" t="s">
         <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10">
         <v>7</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11">
         <v>0.4</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" t="s">
         <v>34</v>
       </c>
       <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11">
         <v>8</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12">
         <v>0.9</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
       <c r="E12" t="s">
         <v>34</v>
       </c>
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12">
         <v>9</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13">
         <v>0.70000000000000007</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
       <c r="E13" t="s">
         <v>34</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14">
         <v>0.2</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
       <c r="E14" t="s">
         <v>34</v>
       </c>
       <c r="F14" t="s">
         <v>34</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>0.2</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
-        <v>34</v>
-      </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
       <c r="F15" t="s">
         <v>34</v>
       </c>
-      <c r="G15">
-        <v>2</v>
+      <c r="G15" t="s">
+        <v>34</v>
       </c>
       <c r="H15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="I15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16">
         <v>0.2</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>34</v>
-      </c>
       <c r="E16" t="s">
         <v>34</v>
       </c>
       <c r="F16" t="s">
         <v>34</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17">
         <v>0.2</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
       <c r="E17" t="s">
         <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>34</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>0.4</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18">
         <v>5</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19">
         <v>0.9</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19">
         <v>6</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
       <c r="F20" t="s">
         <v>34</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20">
         <v>7</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21">
         <v>0.5</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>34</v>
-      </c>
       <c r="E21" t="s">
         <v>34</v>
       </c>
       <c r="F21" t="s">
         <v>34</v>
       </c>
-      <c r="G21">
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21">
         <v>8</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22">
         <v>0.1</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
-        <v>34</v>
-      </c>
       <c r="E22" t="s">
         <v>34</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
       </c>
-      <c r="G22">
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22">
         <v>9</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23">
         <v>0.1</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
       <c r="E23" t="s">
         <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>34</v>
       </c>
-      <c r="G23">
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23">
         <v>10</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24">
         <v>0.8</v>
       </c>
-      <c r="C24" s="10">
+      <c r="D24" s="10">
         <v>1</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E24" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="10">
         <v>1</v>
       </c>
-      <c r="H24" s="10">
+      <c r="I24" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25">
         <v>0.4</v>
       </c>
-      <c r="C25" s="10">
+      <c r="D25" s="10">
         <v>1</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E25" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="10">
         <v>2</v>
       </c>
-      <c r="H25" s="10">
+      <c r="I25" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26">
         <v>0.5</v>
       </c>
-      <c r="C26" s="10">
+      <c r="D26" s="10">
         <v>1</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E26" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="10">
-        <v>3</v>
+      <c r="G26" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="H26" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27">
+      <c r="I26" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27">
         <v>0.5</v>
       </c>
-      <c r="C27" s="10">
+      <c r="D27" s="10">
         <v>1</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E27" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="10">
         <v>4</v>
       </c>
-      <c r="H27" s="10">
+      <c r="I27" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28">
         <v>0.5</v>
       </c>
-      <c r="C28" s="10">
+      <c r="D28" s="10">
         <v>1</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E28" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="10">
         <v>5</v>
       </c>
-      <c r="H28" s="10">
+      <c r="I28" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29">
         <v>0.2</v>
       </c>
-      <c r="C29" s="10">
+      <c r="D29" s="10">
         <v>1</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E29" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="10">
         <v>6</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I29" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C30" s="10">
+      <c r="D30" s="10">
         <v>1</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E30" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F30" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="10">
         <v>7</v>
       </c>
-      <c r="H30" s="10">
+      <c r="I30" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31">
         <v>0.5</v>
       </c>
-      <c r="C31" s="10">
+      <c r="D31" s="10">
         <v>1</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E31" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="10">
         <v>8</v>
       </c>
-      <c r="H31" s="10">
+      <c r="I31" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32">
         <v>0.30000000000000004</v>
       </c>
-      <c r="C32" s="10">
+      <c r="D32" s="10">
         <v>1</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E32" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="10">
         <v>9</v>
       </c>
-      <c r="H32" s="10">
+      <c r="I32" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33">
         <v>0.1</v>
       </c>
-      <c r="C33" s="10">
+      <c r="D33" s="10">
         <v>1</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="E33" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F33" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G33" s="10">
+      <c r="G33" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="10">
         <v>10</v>
       </c>
-      <c r="H33" s="10">
+      <c r="I33" s="10">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
auth functional. routes refactor with req.user
</commit_message>
<xml_diff>
--- a/seed.xlsx
+++ b/seed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharymargolies/Desktop/coding/coding-question-trivia-server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1D871A-0B19-5E40-9F99-4DEFC33D139E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FE1861-4A83-9547-A808-A4426DA9EF8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="topics" sheetId="4" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3687" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3699" uniqueCount="418">
   <si>
     <t>id</t>
   </si>
@@ -1314,6 +1314,9 @@
   </si>
   <si>
     <t>The 'this' keyword refers to a fuction's invocation context.</t>
+  </si>
+  <si>
+    <t>FILLER FACT</t>
   </si>
 </sst>
 </file>
@@ -2577,18 +2580,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:L207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91:J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="65.6640625" customWidth="1"/>
-    <col min="5" max="5" width="72.83203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="72.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.2">
@@ -5122,220 +5125,328 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C91" s="2">
         <v>89</v>
       </c>
+      <c r="D91" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E91" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G91">
+        <v>0.1</v>
+      </c>
       <c r="H91" t="s">
         <v>34</v>
       </c>
       <c r="I91" t="s">
         <v>34</v>
+      </c>
+      <c r="J91" s="2">
+        <v>10</v>
       </c>
       <c r="L91">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C92" s="2">
         <v>90</v>
       </c>
+      <c r="D92" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E92" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G92">
+        <v>0.1</v>
+      </c>
       <c r="H92" t="s">
         <v>34</v>
       </c>
       <c r="I92" t="s">
         <v>34</v>
+      </c>
+      <c r="J92" s="2">
+        <v>11</v>
       </c>
       <c r="L92">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C93" s="2">
         <v>91</v>
       </c>
+      <c r="D93" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E93" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G93">
+        <v>0.1</v>
+      </c>
       <c r="H93" t="s">
         <v>34</v>
       </c>
       <c r="I93" t="s">
         <v>34</v>
+      </c>
+      <c r="J93" s="2">
+        <v>12</v>
       </c>
       <c r="L93">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C94" s="2">
         <v>92</v>
       </c>
+      <c r="D94" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E94" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G94">
+        <v>0.1</v>
+      </c>
       <c r="H94" t="s">
         <v>34</v>
       </c>
       <c r="I94" t="s">
         <v>34</v>
+      </c>
+      <c r="J94" s="2">
+        <v>13</v>
       </c>
       <c r="L94">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C95" s="2">
         <v>93</v>
       </c>
+      <c r="D95" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E95" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G95">
+        <v>0.1</v>
+      </c>
       <c r="H95" t="s">
         <v>34</v>
       </c>
       <c r="I95" t="s">
         <v>34</v>
+      </c>
+      <c r="J95" s="2">
+        <v>14</v>
       </c>
       <c r="L95">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C96" s="2">
         <v>94</v>
       </c>
+      <c r="D96" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E96" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G96">
+        <v>0.1</v>
+      </c>
       <c r="H96" t="s">
         <v>34</v>
       </c>
       <c r="I96" t="s">
         <v>34</v>
+      </c>
+      <c r="J96" s="2">
+        <v>15</v>
       </c>
       <c r="L96">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C97" s="2">
         <v>95</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G97">
+        <v>0.1</v>
+      </c>
       <c r="H97" t="s">
         <v>34</v>
       </c>
       <c r="I97" t="s">
         <v>34</v>
+      </c>
+      <c r="J97" s="2">
+        <v>16</v>
       </c>
       <c r="L97">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C98" s="2">
         <v>96</v>
       </c>
+      <c r="D98" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E98" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G98">
+        <v>0.1</v>
+      </c>
       <c r="H98" t="s">
         <v>34</v>
       </c>
       <c r="I98" t="s">
         <v>34</v>
+      </c>
+      <c r="J98" s="2">
+        <v>17</v>
       </c>
       <c r="L98">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C99" s="2">
         <v>97</v>
       </c>
+      <c r="D99" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E99" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G99">
+        <v>0.1</v>
+      </c>
       <c r="H99" t="s">
         <v>34</v>
       </c>
       <c r="I99" t="s">
         <v>34</v>
+      </c>
+      <c r="J99" s="2">
+        <v>18</v>
       </c>
       <c r="L99">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C100" s="2">
         <v>98</v>
       </c>
+      <c r="D100" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E100" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G100">
+        <v>0.1</v>
+      </c>
       <c r="H100" t="s">
         <v>34</v>
       </c>
       <c r="I100" t="s">
         <v>34</v>
+      </c>
+      <c r="J100" s="2">
+        <v>7</v>
       </c>
       <c r="L100">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C101" s="2">
         <v>99</v>
       </c>
+      <c r="D101" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E101" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G101">
+        <v>0.1</v>
+      </c>
       <c r="H101" t="s">
         <v>34</v>
       </c>
       <c r="I101" t="s">
         <v>34</v>
+      </c>
+      <c r="J101" s="2">
+        <v>9</v>
       </c>
       <c r="L101">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="3:12" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="3:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C102" s="2">
         <v>100</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>417</v>
+      </c>
       <c r="E102" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G102">
+        <v>0.1</v>
+      </c>
       <c r="H102" t="s">
         <v>34</v>
       </c>
       <c r="I102" t="s">
         <v>34</v>
+      </c>
+      <c r="J102" s="2">
+        <v>8</v>
       </c>
       <c r="L102">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="3:12" x14ac:dyDescent="0.2">
@@ -11126,17 +11237,17 @@
   <dimension ref="B3:J209"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="3" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:J209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="93" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="11" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16977,8 +17088,8 @@
   <dimension ref="B3:F203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H102" sqref="H102"/>
+      <pane ySplit="3" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:F203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20410,9 +20521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B3:I415"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D423" sqref="D423"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4:I415"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>